<commit_message>
implementacion acabada de matricula de laboratorio
</commit_message>
<xml_diff>
--- a/siscad/datos/TablaProfesores.xlsx
+++ b/siscad/datos/TablaProfesores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,17 +436,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>dni</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>nombre</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>email</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>dni</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Alvaro Henry Mamani Aliaga</t>
+          <t>41970248</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>amamaniali@unsa.edu.pe</t>
+          <t>LINARES DELGADO, ROLANDO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>41751906</t>
+          <t>rlinaresd@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -478,17 +478,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ana Maria Cuadros Valdivia</t>
+          <t>48064373</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>acuadrosv@unsa.edu.pe</t>
+          <t>QUISPE CRUZ, MARCELA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>29421859</t>
+          <t>mquispecr@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -498,17 +498,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Benigno Erick Sanz Sanz</t>
+          <t>40738010</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>bsanzs@unsa.edu.pe</t>
+          <t>SARMIENTO CALISAYA, EDGAR</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>29641432</t>
+          <t>esarmientoca@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -518,17 +518,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cristian Jose Lopez Del Alamo</t>
+          <t>41751906</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>clopezd@unsa.edu.pe</t>
+          <t>MAMAN ALIAGA, ALVARO HENRY</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>29708892</t>
+          <t>amamaniali@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -538,17 +538,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Edgar Sarmiento Calisaya</t>
+          <t>43185022</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>esarmientoca@unsa.edu.pe</t>
+          <t>HINOJOSA CARDENAS, EDWARD</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>40738010</t>
+          <t>ehinojosa@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -558,17 +558,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Edward Hinojosa Cardenas</t>
+          <t>42397113</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ehinojosa@unsa.edu.pe</t>
+          <t>FLORES QUISPE, ROXANA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>43185022</t>
+          <t>rfloresqu@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -578,17 +578,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Eliana Maria Adriazola Herrera</t>
+          <t>01343039</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>eadriazola@unsa.edu.pe</t>
+          <t>VELAZCO PAREDES, YUBER ELMER</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>40454472</t>
+          <t>yvelazco@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -598,17 +598,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Erika Patricia Lazo Alarcon</t>
+          <t>29579611</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>elazoal@unsa.edu.pe</t>
+          <t>VALDIVIA MALAGA, MARCO ANTONIO</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>29610235</t>
+          <t>mvaldiviama@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -618,17 +618,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Franci Suni Lopez</t>
+          <t>29421859</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>fsunilo@unsa.edu.pe</t>
+          <t>CUADROS VALDIVIA, ANA MARIA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>70616223</t>
+          <t>acuadrosv@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -638,17 +638,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Jesus Heraclio Zuñiga Cueva</t>
+          <t>45622372</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>jzuniga@unsa.edu.pe</t>
+          <t>CARDENAS TALAVERA, ROLANDO JESUS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>29281201</t>
+          <t>rcardenastal@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -658,17 +658,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Jhon Franky Bernedo Gonzales</t>
+          <t>42744760</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>jbernedo@unsa.edu.pe</t>
+          <t>YARI RAMOS, YESSENIA DEYSI</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>41254968</t>
+          <t>yyarira@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -678,17 +678,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Juan Carlos Gutierrez Caceres</t>
+          <t>29525079</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>jgutierrezca@unsa.edu.pe</t>
+          <t>RAMOS LOVON, WILBER ROBERTO</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>30677357</t>
+          <t>wramos@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -698,17 +698,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Judith Hayde Cruz Torres</t>
+          <t>29278874</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>jcruzto@unsa.edu.pe</t>
+          <t>DELGADO BARRA, LUCY ANGELA</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>04438647</t>
+          <t>ldelgado@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -718,17 +718,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Lucy Angela Delgado Barra</t>
+          <t>29281201</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ldelgado@unsa.edu.pe</t>
+          <t>ZUÑIGA CUEVA, JESUS HERACLIO</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>29278874</t>
+          <t>jzuniga@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -738,17 +738,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Marcela Quispe Cruz</t>
+          <t>29610235</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>mquispecr@unsa.edu.pe</t>
+          <t>LAZO ALARCON, ERIKA PATRICIA</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>48064373</t>
+          <t>elazoal@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -758,17 +758,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Marco Antonio Valdivia Malaga</t>
+          <t>30677357</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>mvaldiviama@unsa.edu.pe</t>
+          <t>GUTIERREZ CACERES, JUAN CARLOS</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>29579611</t>
+          <t>jgutierrezca@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -778,17 +778,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Raquel Noelia Arredondo Choque</t>
+          <t>40454472</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>rarredondoc@unsa.edu.pe</t>
+          <t>ADRIANZOLA HERRERA, ELIANA MARIA</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>47493364</t>
+          <t>eadriazola@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -798,17 +798,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Roxana Flores Quispe</t>
+          <t>80000000</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>rfloresqu@unsa.edu.pe</t>
+          <t>CALLOAPAZA PARI, SONIA BENILDA</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>42397113</t>
+          <t>scallcapaza@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -818,17 +818,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Wilber Roberto Ramos Lovon</t>
+          <t>80000001</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>wramos@unsa.edu.pe</t>
+          <t>VILLAR GARNICA, ELVA EMELINA</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>29525079</t>
+          <t>evillar@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -838,17 +838,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Yessenia Deysi Yari Ramos</t>
+          <t>80000002</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>yyarira@unsa.edu.pe</t>
+          <t>SUAREZ LOPEZ, ERNESTO MAURO</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>42744760</t>
+          <t>esuarezlo@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -858,17 +858,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Yuber Elmer Velazco Paredes</t>
+          <t>80000003</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>yvelazco@unsa.edu.pe</t>
+          <t>VERA SAMCHO, JULIO AUGUSTO</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>01343039</t>
+          <t>jveras@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -878,17 +878,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Alberto Garcia Garcia</t>
+          <t>80000004</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>agarciaga@unsa.edu.pe</t>
+          <t>ZAPANA HUMANI, MARY ELIZABETH</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>03375448</t>
+          <t>mzapanahua@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -898,17 +898,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Alex Josue Florez Farfan</t>
+          <t>80000005</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>aflorez@unsa.edu.pe</t>
+          <t>RODRIGUEZ GONZALEZ, PEDRO ALEX</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>41321232</t>
+          <t>prodriguez@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -918,17 +918,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Alvaro Ernesto Cuno Parari</t>
+          <t>80000006</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>acunopa@unsa.edu.pe</t>
+          <t>MAYTA SALAS, ALEJANDRO RAFAEL</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>29692413</t>
+          <t>amaytas@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -938,17 +938,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Angel Eusebio Pilco Escobedo</t>
+          <t>80000007</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>apilcoe@unsa.edu.pe</t>
+          <t>NUÑEZ NUÑEZ, MARIANNY</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>29558780</t>
+          <t>munreznu@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -958,17 +958,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Anny Fresia Centeno Andia</t>
+          <t>80000008</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>acentenoa@unsa.edu.pe</t>
+          <t>CERECEDA QUINTAMILLA, YAKELIN VANESSA</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>40123049</t>
+          <t>ycereceda@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -978,17 +978,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Brayan Adolfo Mujica Guzman</t>
+          <t>80000009</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>bmujica@unsa.edu.pe</t>
+          <t>PEÑALVA SUCA, LORENZO JESUS</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>47353512</t>
+          <t>lpenalvas@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -998,17 +998,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Edson Francisco Luque Mamani</t>
+          <t>80000010</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>eluquem@unsa.edu.pe</t>
+          <t>MALDONADO QUISPE, PERCY</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>45513112</t>
+          <t>pmaldonado@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1018,17 +1018,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Eliseo Daniel Velasquez Condori</t>
+          <t>80000011</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>evelasquezcon@unsa.edu.pe</t>
+          <t>PAZ VALDERBAMA, ALFREDO</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>29594470</t>
+          <t>apazy@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1038,17 +1038,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Erech Ordoñez Ramos</t>
+          <t>80000012</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>eordonez@unsa.edu.pe</t>
+          <t>MESTAS CHAVEZ, ROGER EDWAR</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>01341256</t>
+          <t>rmestasc@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1058,17 +1058,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Evelyn Perez Cervantes</t>
+          <t>80000013</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>eperezce@unsa.edu.pe</t>
+          <t>VIZA HUAYLLASO, JUDID CARINA</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>42790180</t>
+          <t>jvizah@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1078,17 +1078,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Franklin Luis Antonio Cruz Gamero</t>
+          <t>80000014</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>fcruz@unsa.edu.pe</t>
+          <t>OLANDA VELASQUEZ, BERTHA</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>42932629</t>
+          <t>bolanda@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1098,17 +1098,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Grover Enrique Castro Guzman</t>
+          <t>80000015</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>gcastrogu@unsa.edu.pe</t>
+          <t>QUISPE MAMANI, ANTONIA</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>72802217</t>
+          <t>aquisperm@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1118,17 +1118,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Guadalupe Del Rosario Quispe Saji</t>
+          <t>80000016</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>gquispesaj@unsa.edu.pe</t>
+          <t>LUQUE FERNANDEZ, CESAR RAUL</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>29707257</t>
+          <t>cluquef@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1138,17 +1138,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Jesus Enrique Achire Quispe</t>
+          <t>80000017</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>jachire@unsa.edu.pe</t>
+          <t>AQUISE ESCOBEDO, SERGIO MOISES</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>44203864</t>
+          <t>saquisee@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1158,17 +1158,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Jorge Antonio Ihue Umire</t>
+          <t>80000018</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>jihue@unsa.edu.pe</t>
+          <t>ROQUE ROJI, ELIANA</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>40882165</t>
+          <t>eroquero@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1178,17 +1178,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Juan Carlos Zuñiga Torres</t>
+          <t>80000019</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>jzunigat@unsa.edu.pe</t>
+          <t>CONDORI ROCA, WILLY</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>43254657</t>
+          <t>wcondorir@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1198,17 +1198,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Julio Raul Medina Cruz</t>
+          <t>80000020</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>jmedinacr@unsa.edu.pe</t>
+          <t>MORALES MOYA, ADHA</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>46275182</t>
+          <t>amoralesmo@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1218,17 +1218,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Marina Jeaneth Machicao Justo</t>
+          <t>80000021</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>mmachicaoj@unsa.edu.pe</t>
+          <t>HANCO ANCORI, RICARDO JAVIER</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>43704362</t>
+          <t>rhancoan@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1238,17 +1238,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Marisol Cristel Galarza Flores</t>
+          <t>80000022</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>mgalarza@unsa.edu.pe</t>
+          <t>CANO MAMANI, ADELA LUISA</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>43518581</t>
+          <t>acanoma@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1258,17 +1258,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Milton Raul Condori Fernandez</t>
+          <t>80000023</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>mcondorife@unsa.edu.pe</t>
+          <t>CABANA HANCO, WILSON RICARDO</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>47316290</t>
+          <t>wcabana@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1278,17 +1278,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Pablo Cesar Calcina Ccori</t>
+          <t>80000024</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>pcalcinacc@unsa.edu.pe</t>
+          <t>VELAZCO COACYAHUILLCA, YSIDRO</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>42426051</t>
+          <t>yvelazcoco@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1298,17 +1298,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Percy Antonio Ticona Centeno</t>
+          <t>80000025</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>pticonac@unsa.edu.pe</t>
+          <t>GUTIERREZ RODRIGUEZ, EDDY AUGUSTO</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>29540131</t>
+          <t>egutierrezro@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1318,17 +1318,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Reynaldo Ricardo Quispe Infantes</t>
+          <t>80000026</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>rquispein@unsa.edu.pe</t>
+          <t>VELASQUEZ CONDORI, ELISEO DANIEL</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>42000770</t>
+          <t>evelasquezcon@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1338,17 +1338,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Rolando Jesus Cardenas Talavera</t>
+          <t>80000027</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>rcardenastal@unsa.edu.pe</t>
+          <t>CACERES ANCO, ROBERTO</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>45622372</t>
+          <t>rcaceresa@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1358,17 +1358,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Rolando Linares Delgado</t>
+          <t>80000028</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>rlinaresd@unsa.edu.pe</t>
+          <t>JACOBE AGUIRRE, ROCIO</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>41970248</t>
+          <t>rjacobe@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1378,17 +1378,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Ronny Ivan Gonzales Medina</t>
+          <t>80000029</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>rgonzalesme@unsa.edu.pe</t>
+          <t>PILCO ANDIA, CARLOTA CRISTINA</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>29731966</t>
+          <t>cpilcoa@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1398,20 +1398,300 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Yesica Karin Granda Lazaro</t>
+          <t>80000030</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ygranda@unsa.edu.pe</t>
+          <t>OSORIO MENDOZA DE MONTEZA, NADJA CATALINA</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>09677923</t>
+          <t>nosoriom@unsa.edu.pe</t>
         </is>
       </c>
       <c r="D49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>80000031</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ZEBALLOS RAMIREZ, PIAR ELIZABETH</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>pzeballosra@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>80000032</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MESTAS VALDIVIA, JOSE CARLOS</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>jmestasv@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>80000033</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>MONROY CARNERO, DANIEL JESUS</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>dmonroyc@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>80000034</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>TACCA QUISPE, LORENZO WILBERT</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ltacca@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>80000035</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>TORRES GONZALES, SELENE BELEN</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>storresg@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>80000036</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>NUÑEZ GUZMAN, ROXANA LUISA</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>rnunezg@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>80000037</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>CALLO HUAYNA, JENNY LAURA</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>jcalloh@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>80000038</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>GARCIA QUISPE, WILLY ENRIQUE</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>wgarcia@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>80000039</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>CHIRINOS TOVAR, KARINA ROGELIO</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>kchirinost@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>80000040</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>CACERES CAERO, FELIX</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>fcaceresca@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>80000041</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>BUSTAMANTE LOPEZ, TEIS LARISA</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>tbustamante@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>80000042</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>CORDOVA MARTINEZ, MARIA DEL CARMEN</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>mcordovam@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>80000043</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>QUISPE MELON, MILAGROS</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>mquispemel@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>80000044</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>CAHUANA MONTERO, GARY MARY</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>gcahuana@unsa.edu.pe</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>